<commit_message>
Second commit to show pengajuan cash rewards
</commit_message>
<xml_diff>
--- a/DB_MasterPeriode.xlsx
+++ b/DB_MasterPeriode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Katalon Studio\ACCPartner-CMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114CA773-84BE-4875-803A-F18615E8724B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530B64FC-68BC-458C-9294-FCF349B6D65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{65B442A5-349C-43E6-9C47-35AB4AF3A557}"/>
   </bookViews>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>varPeriodeMulai</t>
-  </si>
-  <si>
-    <t>varPeriodeSelesai</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>varBenar</t>
   </si>
@@ -43,16 +34,49 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>varUsername</t>
+  </si>
+  <si>
+    <t>varPassword</t>
+  </si>
+  <si>
+    <t>varMulai</t>
+  </si>
+  <si>
+    <t>varSelesai</t>
+  </si>
+  <si>
+    <t>varSearch</t>
+  </si>
+  <si>
+    <t>varUbahSelesai</t>
+  </si>
+  <si>
+    <t>gilank.rangesti</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>HJKL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,63 +421,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED828AA4-F8DD-4B8D-9C78-408602C83DAD}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>202009</v>
+      </c>
+      <c r="D2" s="1">
+        <v>202109</v>
+      </c>
+      <c r="E2" s="1">
+        <v>202009</v>
+      </c>
+      <c r="F2" s="1">
+        <v>202110</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>201902</v>
-      </c>
-      <c r="B2" s="1">
-        <v>202002</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>202008</v>
+      </c>
+      <c r="D3" s="1">
+        <v>202108</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>202109</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2020</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>